<commit_message>
Added README for contentOptimizer
</commit_message>
<xml_diff>
--- a/Documents/Testplan.xlsx
+++ b/Documents/Testplan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="300" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestPlan" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="108">
   <si>
     <t>Test Planner and Tracker</t>
   </si>
@@ -124,7 +124,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Graphs get rendered and </t>
+      <t>Graphs get rendered and </t>
     </r>
     <r>
       <rPr>
@@ -132,41 +132,64 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">updated</t>
+      <t>updated</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> correctly</t>
+      <t> correctly</t>
     </r>
   </si>
   <si>
     <t>Basic SQL execution on NGINX server</t>
   </si>
   <si>
+    <t>Availibility of an up and running nginx server with MySQL configured.</t>
+  </si>
+  <si>
+    <t>1) Basic SQL queries(SELECT, INSERT etc.) are written.                                                     2) They are executed using php on the server database.</t>
+  </si>
+  <si>
+    <t>Data is retrieved from/written into various tables.</t>
+  </si>
+  <si>
     <t>Testing if unique global visitor ID is generated.</t>
   </si>
   <si>
+    <t>The unique guid function should have been written.</t>
+  </si>
+  <si>
+    <t>1) A console.log() is done on the visitor id variable.</t>
+  </si>
+  <si>
+    <t>The visitor id is printed on the browser console.</t>
+  </si>
+  <si>
     <t>Testing http post request sent to server.</t>
   </si>
   <si>
+    <t>An up an running server.</t>
+  </si>
+  <si>
+    <t>1) An AJAX POST request is sent to the server with success and failure response functions.</t>
+  </si>
+  <si>
+    <t>Success response function is executed.</t>
+  </si>
+  <si>
+    <t>Cross-origin requests are disallowed by servers by default. CORS needs to be enabled.</t>
+  </si>
+  <si>
     <t>Testing Http post request sent to user after enabling CORS.</t>
   </si>
   <si>
-    <t>Testing for datapub load time.</t>
-  </si>
-  <si>
-    <t>Testing for datapub load time(after enabling asynchronous call).</t>
-  </si>
-  <si>
-    <t>Checking testing for recently viewed articles.</t>
-  </si>
-  <si>
-    <t>Testing SQL query for getting scores for a particular user for a particular URL.</t>
+    <t>An up an running server. CORS should be enabled.</t>
   </si>
   <si>
     <t>Checking if a given visit date was within the range defined by the date filter.</t>
@@ -373,11 +396,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -395,121 +419,11 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFF20884"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FFFF9900"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="11"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006411"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="15"/>
-      <color rgb="FF003366"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="13"/>
-      <color rgb="FF003366"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF003366"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF333399"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF9900"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF993300"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="18"/>
-      <color rgb="FF003366"/>
-      <name val="Cambria"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFDD0806"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="16"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -517,32 +431,44 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF00000A"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -551,122 +477,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FF009933"/>
+        <bgColor rgb="FF1FB714"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFDD0806"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCFF"/>
-        <bgColor rgb="FFC0C0C0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFFF"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF99CCFF"/>
-        <bgColor rgb="FFCCCCFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC99FF"/>
-        <bgColor rgb="FF9999FF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0066CC"/>
-        <bgColor rgb="FF008080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF8080"/>
-        <bgColor rgb="FFFF99CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC0C0C0"/>
-        <bgColor rgb="FFCCCCFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF33CCCC"/>
-        <bgColor rgb="FF00CCFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF333399"/>
-        <bgColor rgb="FF3C3C3C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF90713A"/>
-        <bgColor rgb="FF808080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF800080"/>
-        <bgColor rgb="FF800080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF99CC"/>
-        <bgColor rgb="FFFF8080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF969696"/>
-        <bgColor rgb="FF808080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF009933"/>
-        <bgColor rgb="FF1FB714"/>
       </patternFill>
     </fill>
     <fill>
@@ -678,11 +502,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDD0806"/>
-        <bgColor rgb="FFF20884"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="13">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -692,113 +516,6 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="double">
-        <color rgb="FF333333"/>
-      </left>
-      <right style="double">
-        <color rgb="FF333333"/>
-      </right>
-      <top style="double">
-        <color rgb="FF333333"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF333333"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color rgb="FF333399"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color rgb="FFC0C0C0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF0066CC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF9900"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FFC0C0C0"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFC0C0C0"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFC0C0C0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFC0C0C0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF333333"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF333333"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF333333"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF333333"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF333399"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF333399"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
         <color rgb="FF3C3C3C"/>
       </left>
       <right style="thin">
@@ -938,7 +655,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -962,49 +679,8 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="11" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="13" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="14" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="15" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="16" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="11" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="17" borderId="2" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="18" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="16" fillId="19" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="20" borderId="7" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="8" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="9" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="56">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1013,27 +689,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1041,43 +717,59 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="21" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1085,63 +777,63 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="22" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="22" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1161,124 +853,83 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="22" borderId="20" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="23" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="22" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="22" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="20% - Accent1" xfId="20" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="20% - Accent2" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="20% - Accent3" xfId="22" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="20% - Accent4" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="20% - Accent5" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="20% - Accent6" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="40% - Accent1" xfId="26" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="40% - Accent2" xfId="27" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="40% - Accent4" xfId="29" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="40% - Accent5" xfId="30" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="40% - Accent6" xfId="31" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="60% - Accent1" xfId="32" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="60% - Accent2" xfId="33" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="60% - Accent3" xfId="34" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="60% - Accent4" xfId="35" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="60% - Accent5" xfId="36" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="60% - Accent6" xfId="37" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Accent1" xfId="38" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Accent2" xfId="39" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Accent3" xfId="40" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Accent4" xfId="41" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Accent5" xfId="42" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Accent6" xfId="43" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="44" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Calculation" xfId="45" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Check Cell" xfId="46" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Explanatory Text" xfId="47" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="48" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="49" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="50" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Heading 3" xfId="51" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Heading 4" xfId="52" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Input" xfId="53" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Linked Cell" xfId="54" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="55" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="56" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Output" xfId="57" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Title" xfId="58" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Total" xfId="59" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Warning Text" xfId="60" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFDD0806"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFF20884"/>
+      <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006411"/>
+      <rgbColor rgb="FF009933"/>
       <rgbColor rgb="FF00000A"/>
-      <rgbColor rgb="FF90713A"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF009933"/>
+      <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
@@ -1316,11 +967,11 @@
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF1FB714"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF3C3C3C"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FFDD0806"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF3C3C3C"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1333,8 +984,8 @@
   </sheetPr>
   <dimension ref="A1:I65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q14" activeCellId="0" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -1527,7 +1178,7 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="n">
         <f aca="false">A8+1</f>
         <v>7</v>
@@ -1535,160 +1186,141 @@
       <c r="B9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
+      <c r="C9" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>37</v>
+      </c>
       <c r="F9" s="15"/>
       <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+      <c r="H9" s="12"/>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="n">
         <v>8</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
+        <v>38</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>41</v>
+      </c>
       <c r="F10" s="15"/>
       <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="H10" s="12"/>
       <c r="I10" s="14"/>
     </row>
-    <row r="11" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="n">
         <v>9</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
+        <v>42</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F11" s="15"/>
       <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-    </row>
-    <row r="12" customFormat="false" ht="36.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H11" s="17"/>
+      <c r="I11" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="n">
         <v>10</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
+        <v>47</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F12" s="15"/>
       <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="H12" s="12"/>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+        <v>49</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="18"/>
       <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="H13" s="12"/>
       <c r="I13" s="14"/>
     </row>
-    <row r="14" customFormat="false" ht="36.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
+        <v>53</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="19"/>
       <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="H14" s="12"/>
       <c r="I14" s="14"/>
     </row>
-    <row r="15" customFormat="false" ht="36.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-    </row>
-    <row r="16" customFormat="false" ht="47.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-    </row>
-    <row r="17" customFormat="false" ht="47.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-    </row>
-    <row r="18" customFormat="false" ht="58.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0"/>
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13"/>
@@ -1870,83 +1502,83 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="16" t="s">
-        <v>50</v>
+      <c r="B1" s="20" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="17" t="s">
-        <v>51</v>
+      <c r="B3" s="21" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="17" t="s">
-        <v>52</v>
+      <c r="B4" s="21" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="17" t="s">
-        <v>53</v>
+      <c r="B5" s="21" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="17" t="s">
-        <v>54</v>
+      <c r="B6" s="21" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="17" t="s">
-        <v>55</v>
+      <c r="B7" s="21" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="17" t="s">
-        <v>56</v>
+      <c r="B8" s="21" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="17" t="s">
-        <v>57</v>
+      <c r="B9" s="21" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="17" t="s">
-        <v>58</v>
+      <c r="B10" s="21" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="17" t="s">
-        <v>59</v>
+      <c r="B11" s="21" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="17" t="s">
-        <v>60</v>
+      <c r="B12" s="21" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="17" t="s">
-        <v>61</v>
+      <c r="B13" s="21" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="17" t="s">
-        <v>62</v>
+      <c r="B14" s="21" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="17" t="s">
-        <v>63</v>
+      <c r="B15" s="21" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="17" t="s">
-        <v>64</v>
+      <c r="B16" s="21" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="17" t="s">
-        <v>65</v>
+      <c r="B17" s="21" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1985,32 +1617,32 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
+      <c r="A2" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
-      <c r="B3" s="19" t="s">
-        <v>67</v>
+      <c r="B3" s="23" t="s">
+        <v>74</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="0" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
+      <c r="A5" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
@@ -2018,195 +1650,195 @@
       <c r="C6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="23" t="s">
+      <c r="A7" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>75</v>
+      <c r="F7" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24" t="n">
+      <c r="A8" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="B8" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="29"/>
+      <c r="B8" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="G8" s="33"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="n">
+      <c r="A9" s="34" t="n">
         <v>2</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="F9" s="34"/>
-      <c r="G9" s="29"/>
+      <c r="B9" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="38"/>
+      <c r="G9" s="33"/>
     </row>
     <row r="10" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="35" t="n">
+      <c r="A10" s="39" t="n">
         <v>3</v>
       </c>
-      <c r="B10" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="F10" s="39"/>
-      <c r="G10" s="40"/>
+      <c r="B10" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
     </row>
     <row r="11" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="F11" s="41"/>
-      <c r="G11" s="42"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" s="45"/>
+      <c r="G11" s="46"/>
     </row>
     <row r="12" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="43" t="n">
+      <c r="A12" s="47" t="n">
         <v>4</v>
       </c>
-      <c r="B12" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="D12" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="E12" s="46" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="47"/>
-      <c r="G12" s="48"/>
+      <c r="B12" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="51"/>
+      <c r="G12" s="52"/>
     </row>
     <row r="13" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="24"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="E13" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="42"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="32"/>
+      <c r="G13" s="46"/>
     </row>
     <row r="14" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="43" t="n">
+      <c r="A14" s="47" t="n">
         <v>5</v>
       </c>
-      <c r="B14" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="D14" s="45" t="s">
+      <c r="B14" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="46" t="s">
+      <c r="C14" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="51"/>
+      <c r="G14" s="52"/>
+    </row>
+    <row r="15" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" s="46"/>
+    </row>
+    <row r="16" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="47" t="n">
+        <v>6</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="F14" s="47"/>
-      <c r="G14" s="48"/>
-    </row>
-    <row r="15" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="E15" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="F15" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="G15" s="42"/>
-    </row>
-    <row r="16" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="43" t="n">
-        <v>6</v>
-      </c>
-      <c r="B16" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" s="45" t="s">
+      <c r="D16" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="F16" s="54"/>
+      <c r="G16" s="52"/>
+    </row>
+    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="F16" s="50"/>
-      <c r="G16" s="48"/>
-    </row>
-    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="24"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="E17" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="F17" s="51"/>
-      <c r="G17" s="42"/>
+      <c r="E17" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17" s="55"/>
+      <c r="G17" s="46"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>